<commit_message>
updated bandiwidth memory comparison files to include spherical and group by cov type
</commit_message>
<xml_diff>
--- a/benchmarks/bandwidth_comparison.xlsx
+++ b/benchmarks/bandwidth_comparison.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>diag</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -504,16 +504,16 @@
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2550887025215122</v>
+        <v>0.7015744201314714</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5416756271900819</v>
+        <v>0.701546223192952</v>
       </c>
       <c r="I2" t="n">
-        <v>112.347948707921</v>
+        <v>-0.004019094441060897</v>
       </c>
       <c r="J2" t="n">
-        <v>0.154876708984375</v>
+        <v>0.1541900634765625</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -534,29 +534,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>tied</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>1000</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1981012679313282</v>
+        <v>1.134292682909713</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1686512483484929</v>
+        <v>0.5726330390366123</v>
       </c>
       <c r="I3" t="n">
-        <v>-14.86614391233685</v>
+        <v>-49.5162890791395</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1594924926757812</v>
+        <v>0.3853607177734375</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -577,29 +577,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>1000</v>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
         <v>5</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2157318997521248</v>
+        <v>1.34721696365025</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1322019511287935</v>
+        <v>0.9428173016857128</v>
       </c>
       <c r="I4" t="n">
-        <v>-38.71933113244118</v>
+        <v>-30.0174116623967</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1839065551757812</v>
+        <v>0.7706451416015625</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -620,29 +620,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>diag</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>10000</v>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
       </c>
       <c r="G5" t="n">
-        <v>0.235768653212597</v>
+        <v>0.975233274288575</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2916142672280241</v>
+        <v>0.6089120631963344</v>
       </c>
       <c r="I5" t="n">
-        <v>23.68661535554944</v>
+        <v>-37.56241924369008</v>
       </c>
       <c r="J5" t="n">
-        <v>3.820419311523438</v>
+        <v>1.527481079101562</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -663,7 +663,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>tied</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -676,16 +676,16 @@
         <v>5</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1529217762338884</v>
+        <v>0.9065907536609606</v>
       </c>
       <c r="H6" t="n">
-        <v>0.08490281033387501</v>
+        <v>0.893021506445439</v>
       </c>
       <c r="I6" t="n">
-        <v>-44.47958137497751</v>
+        <v>-1.496733466641573</v>
       </c>
       <c r="J6" t="n">
-        <v>3.854789733886719</v>
+        <v>3.818588256835938</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -706,29 +706,29 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>10000</v>
       </c>
       <c r="E7" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2922991149652943</v>
+        <v>0.956117040695989</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3316080007082786</v>
+        <v>1.062239862520369</v>
       </c>
       <c r="I7" t="n">
-        <v>13.44817131849735</v>
+        <v>11.09935471363733</v>
       </c>
       <c r="J7" t="n">
-        <v>4.007377624511719</v>
+        <v>7.637100219726562</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -749,29 +749,29 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>diag</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E8" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2591947804628438</v>
+        <v>0.4173162768993426</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1503487856790492</v>
+        <v>0.4421363213114048</v>
       </c>
       <c r="I8" t="n">
-        <v>-41.99389917861326</v>
+        <v>5.947538063090896</v>
       </c>
       <c r="J8" t="n">
-        <v>7.640838623046875</v>
+        <v>15.26039123535156</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -792,29 +792,29 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>tied</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E9" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1651164803652252</v>
+        <v>0.4725279944489104</v>
       </c>
       <c r="H9" t="n">
-        <v>0.08202483754593139</v>
+        <v>0.4824051627566785</v>
       </c>
       <c r="I9" t="n">
-        <v>-50.32304627345579</v>
+        <v>2.090282147047691</v>
       </c>
       <c r="J9" t="n">
-        <v>7.785835266113281</v>
+        <v>38.15086364746094</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -835,11 +835,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>spherical</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E10" t="n">
         <v>100</v>
@@ -848,16 +848,16 @@
         <v>5</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1984106014512493</v>
+        <v>0.3524692638889246</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1865802368516945</v>
+        <v>0.422992224535525</v>
       </c>
       <c r="I10" t="n">
-        <v>-5.962566774669822</v>
+        <v>20.00825827151402</v>
       </c>
       <c r="J10" t="n">
-        <v>8.396186828613281</v>
+        <v>76.30165100097656</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="E11" t="n">
         <v>20</v>
@@ -891,16 +891,16 @@
         <v>5</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2380001834103861</v>
+        <v>0.258874021942084</v>
       </c>
       <c r="H11" t="n">
-        <v>0.194681652500499</v>
+        <v>0.574277961053328</v>
       </c>
       <c r="I11" t="n">
-        <v>-18.20104938120679</v>
+        <v>121.836844324923</v>
       </c>
       <c r="J11" t="n">
-        <v>15.26107788085938</v>
+        <v>0.154876708984375</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -921,29 +921,29 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>tied</t>
+          <t>diag</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F12" t="n">
         <v>5</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2050105953080839</v>
+        <v>0.3513764414818237</v>
       </c>
       <c r="H12" t="n">
-        <v>0.09224685308864432</v>
+        <v>0.2796338387732188</v>
       </c>
       <c r="I12" t="n">
-        <v>-55.00386067850862</v>
+        <v>-20.41759043550337</v>
       </c>
       <c r="J12" t="n">
-        <v>15.26569366455078</v>
+        <v>0.3871917724609375</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -964,31 +964,1063 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>100</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.2199493453542603</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.2443524013619396</v>
+      </c>
+      <c r="I13" t="n">
+        <v>11.09485275729039</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.774383544921875</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.4174688286418736</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.2686775796295765</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-35.64128356513485</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.528167724609375</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.2879658051317067</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.3345187964961477</v>
+      </c>
+      <c r="I15" t="n">
+        <v>16.16615255521369</v>
+      </c>
+      <c r="J15" t="n">
+        <v>3.820419311523438</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.3153553314314964</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.2061974527666486</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-34.61424868555292</v>
+      </c>
+      <c r="J16" t="n">
+        <v>7.640838623046875</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E17" t="n">
+        <v>20</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.160255769084728</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.1865073259909731</v>
+      </c>
+      <c r="I17" t="n">
+        <v>16.38103704857313</v>
+      </c>
+      <c r="J17" t="n">
+        <v>15.26107788085938</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E18" t="n">
+        <v>50</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2023087776726096</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.1736795936083536</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-14.15123179212017</v>
+      </c>
+      <c r="J18" t="n">
+        <v>38.15269470214844</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>diag</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1942836651273165</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.1497868520127199</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-22.90301301729988</v>
+      </c>
+      <c r="J19" t="n">
+        <v>76.30538940429688</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1093521409556551</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.2031964006389314</v>
+      </c>
+      <c r="I20" t="n">
+        <v>85.81840178267056</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.1594924926757812</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E21" t="n">
+        <v>50</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1847068512326324</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.1534636037819644</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-16.91504524178053</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.4215621948242188</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.2288630146786772</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.1748833470804868</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-23.58601614768453</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.9193801879882812</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E23" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.2641473500576255</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.1737002878179531</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-34.24113935647687</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1.532783508300781</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E24" t="n">
+        <v>50</v>
+      </c>
+      <c r="F24" t="n">
+        <v>5</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2335179721552549</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0811470821554908</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-65.25017693218919</v>
+      </c>
+      <c r="J24" t="n">
+        <v>3.854789733886719</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E25" t="n">
+        <v>100</v>
+      </c>
+      <c r="F25" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1580370718765134</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0619385558089724</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-60.80757820078456</v>
+      </c>
+      <c r="J25" t="n">
+        <v>7.785835266113281</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E26" t="n">
+        <v>20</v>
+      </c>
+      <c r="F26" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1814977296456387</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.08346067485612856</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-54.0155818923578</v>
+      </c>
+      <c r="J26" t="n">
+        <v>15.26569366455078</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E27" t="n">
+        <v>50</v>
+      </c>
+      <c r="F27" t="n">
+        <v>5</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1636982184370287</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.08899407901819283</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-45.63527943804287</v>
+      </c>
+      <c r="J27" t="n">
+        <v>38.18706512451172</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>tied</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E28" t="n">
+        <v>100</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.1439605828650163</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.07476581555263585</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-48.06507860367615</v>
+      </c>
+      <c r="J28" t="n">
+        <v>76.45038604736328</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>full</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E29" t="n">
+        <v>20</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.2239960176936991</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.4151690753938289</v>
+      </c>
+      <c r="I29" t="n">
+        <v>85.34663235019976</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.1839065551757812</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E30" t="n">
+        <v>50</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1951784014888432</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.4144124092162844</v>
+      </c>
+      <c r="I30" t="n">
+        <v>112.324932500266</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.5741500854492188</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E31" t="n">
+        <v>100</v>
+      </c>
+      <c r="F31" t="n">
+        <v>5</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.2600208070220888</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.3894495006973406</v>
+      </c>
+      <c r="I31" t="n">
+        <v>49.77628335114613</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.529731750488281</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E32" t="n">
+        <v>20</v>
+      </c>
+      <c r="F32" t="n">
+        <v>5</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.2728758090506137</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.3780064899980661</v>
+      </c>
+      <c r="I32" t="n">
+        <v>38.52693330098472</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1.557197570800781</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E33" t="n">
+        <v>50</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.2213533125078829</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.2823953755065726</v>
+      </c>
+      <c r="I33" t="n">
+        <v>27.57675604990816</v>
+      </c>
+      <c r="J33" t="n">
+        <v>4.007377624511719</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E34" t="n">
+        <v>100</v>
+      </c>
+      <c r="F34" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.1534202104088854</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.1364918009608922</v>
+      </c>
+      <c r="I34" t="n">
+        <v>-11.03401527274456</v>
+      </c>
+      <c r="J34" t="n">
+        <v>8.396186828613281</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>100000</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E35" t="n">
         <v>20</v>
       </c>
-      <c r="F13" t="n">
-        <v>5</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.1395058231897943</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.2043151182426059</v>
-      </c>
-      <c r="I13" t="n">
-        <v>46.45633678290272</v>
-      </c>
-      <c r="J13" t="n">
+      <c r="F35" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.1845986573545001</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.1966530305119801</v>
+      </c>
+      <c r="I35" t="n">
+        <v>6.530043788092687</v>
+      </c>
+      <c r="J35" t="n">
         <v>15.29010772705078</v>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E36" t="n">
+        <v>50</v>
+      </c>
+      <c r="F36" t="n">
+        <v>5</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.1964264332662506</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.1947985007281829</v>
+      </c>
+      <c r="I36" t="n">
+        <v>-0.8287746771134237</v>
+      </c>
+      <c r="J36" t="n">
+        <v>38.33965301513672</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>_maximization_step</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bandwidth (GB/s)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E37" t="n">
+        <v>100</v>
+      </c>
+      <c r="F37" t="n">
+        <v>5</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.1660262658549497</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.1698593220442388</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2.308704691725041</v>
+      </c>
+      <c r="J37" t="n">
+        <v>77.06073760986328</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>cpu</t>
         </is>

</xml_diff>